<commit_message>
implement delete plan activity
</commit_message>
<xml_diff>
--- a/public/Site Template.xlsx
+++ b/public/Site Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kuliah\Magang\PKL\Development\frontend-ran-dashboard\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kuliah\PKL\Development\frontend-ran-dashboard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBE5055-0D89-4F95-B5ED-AD34B057B371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C6C96B-AC5A-478B-A225-E5CD45B0A486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -414,7 +425,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>